<commit_message>
coded chonky swordfish effect
</commit_message>
<xml_diff>
--- a/UwUArena/UwUArenaMinions.xlsx
+++ b/UwUArena/UwUArenaMinions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikita/Desktop/UwUArena/UwUArena/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{12008979-8AA8-6940-A50F-27D8FD597211}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5614122C-0630-7C48-9E79-AA18C16814F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F230C6A4-441C-B04C-941A-03EB20218167}"/>
   </bookViews>
@@ -57,7 +57,7 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Pooka</t>
+    <t>Booka</t>
   </si>
   <si>
     <t>Every time this minions takes damage, give it +1 attack.</t>
@@ -616,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B1918B-2F12-4841-B2D9-4EC4C4CC40F4}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fixed gifts and effects and added wall of flame effect
</commit_message>
<xml_diff>
--- a/UwUArena/UwUArenaMinions.xlsx
+++ b/UwUArena/UwUArenaMinions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikita/Desktop/UwUArena/UwUArena/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{42ACDE63-2C0D-CB41-A8EF-E216AAF2BBB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5C298460-6229-4344-8C83-6465C9739888}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F230C6A4-441C-B04C-941A-03EB20218167}"/>
   </bookViews>
@@ -204,9 +204,6 @@
     <t>Entry: Gift(1) When a forest minion enters, double its stats</t>
   </si>
   <si>
-    <t>Entry: Gift (5) When a pyro minion enters, give it attack equal to this minions hp.</t>
-  </si>
-  <si>
     <t>Entry Gift(3) When a forest minion enters, give it +3/3</t>
   </si>
   <si>
@@ -235,6 +232,9 @@
   </si>
   <si>
     <t xml:space="preserve">On Death: Shuffle an exact copy of this into your roster with x/x where x is this minion's current attack -1. </t>
+  </si>
+  <si>
+    <t>Entry: Gift (2) When a pyro minion enters, give it attack equal to this minions hp.</t>
   </si>
 </sst>
 </file>
@@ -616,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B1918B-2F12-4841-B2D9-4EC4C4CC40F4}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="108" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="108" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -809,7 +809,7 @@
         <v>4</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -969,7 +969,7 @@
         <v>5</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -989,7 +989,7 @@
         <v>5</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -1106,7 +1106,7 @@
         <v>2</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -1186,7 +1186,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -1194,7 +1194,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>45</v>
@@ -1206,7 +1206,7 @@
         <v>2</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -1214,7 +1214,7 @@
         <v>2</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>45</v>
@@ -1226,7 +1226,7 @@
         <v>4</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -1234,7 +1234,7 @@
         <v>3</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>45</v>
@@ -1246,7 +1246,7 @@
         <v>9</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
can instantiate entire game object
</commit_message>
<xml_diff>
--- a/UwUArena/UwUArenaMinions.xlsx
+++ b/UwUArena/UwUArenaMinions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikita/Desktop/UwUArena/UwUArena/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0847EAF0-A6B5-2249-A55F-8208CDAD1222}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0E8AAE1A-E672-3944-B9DA-031F52668DE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F230C6A4-441C-B04C-941A-03EB20218167}"/>
   </bookViews>
@@ -66,9 +66,6 @@
     <t>Chonky Swordfish</t>
   </si>
   <si>
-    <t>Entry: Gift (1): If an aquatic minions enters, give the minion "can't take damage when it attacks".</t>
-  </si>
-  <si>
     <t xml:space="preserve">Death: Trap (1): When a minion enters, set its attack to 0 until it receives damage. </t>
   </si>
   <si>
@@ -253,6 +250,9 @@
   </si>
   <si>
     <t>Death: Add every minion Dunkmaster Dracarius killed to your battle roster.</t>
+  </si>
+  <si>
+    <t>Entry: Gift (1): If an aquatic minions enters, give the minion: can't take damage when it attacks.</t>
   </si>
 </sst>
 </file>
@@ -634,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B1918B-2F12-4841-B2D9-4EC4C4CC40F4}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="108" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -687,7 +687,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -695,7 +695,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -707,7 +707,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -735,7 +735,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
@@ -747,7 +747,7 @@
         <v>4</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -755,7 +755,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>6</v>
@@ -767,7 +767,7 @@
         <v>3</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -775,7 +775,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
@@ -787,7 +787,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -795,7 +795,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
@@ -807,7 +807,7 @@
         <v>12</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -815,7 +815,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>6</v>
@@ -827,7 +827,7 @@
         <v>4</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -835,7 +835,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>6</v>
@@ -847,7 +847,7 @@
         <v>8</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -855,7 +855,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>6</v>
@@ -867,10 +867,10 @@
         <v>8</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -878,19 +878,19 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="1">
-        <v>1</v>
-      </c>
-      <c r="E12" s="1">
-        <v>1</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -898,10 +898,10 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="1">
         <v>2</v>
@@ -910,7 +910,7 @@
         <v>2</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -918,10 +918,10 @@
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" s="1">
         <v>5</v>
@@ -930,7 +930,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -938,19 +938,19 @@
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="1">
+        <v>2</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="1">
-        <v>2</v>
-      </c>
-      <c r="E15" s="1">
-        <v>1</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -958,10 +958,10 @@
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
@@ -970,7 +970,7 @@
         <v>2</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -978,10 +978,10 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
@@ -990,7 +990,7 @@
         <v>5</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -998,10 +998,10 @@
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D18" s="1">
         <v>4</v>
@@ -1010,7 +1010,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -1018,10 +1018,10 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" s="1">
         <v>10</v>
@@ -1030,7 +1030,7 @@
         <v>4</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -1038,10 +1038,10 @@
         <v>3</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D20" s="1">
         <v>8</v>
@@ -1050,7 +1050,7 @@
         <v>8</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -1058,10 +1058,10 @@
         <v>3</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D21" s="1">
         <v>2</v>
@@ -1070,7 +1070,7 @@
         <v>5</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -1078,10 +1078,10 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D22" s="1">
         <v>3</v>
@@ -1095,10 +1095,10 @@
         <v>2</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D23" s="1">
         <v>4</v>
@@ -1107,7 +1107,7 @@
         <v>4</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -1115,10 +1115,10 @@
         <v>3</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D24" s="1">
         <v>2</v>
@@ -1127,7 +1127,7 @@
         <v>2</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -1135,10 +1135,10 @@
         <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D25" s="1">
         <v>6</v>
@@ -1147,7 +1147,7 @@
         <v>6</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -1155,19 +1155,19 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" s="1">
+        <v>5</v>
+      </c>
+      <c r="E26" s="1">
+        <v>5</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" s="1">
-        <v>5</v>
-      </c>
-      <c r="E26" s="1">
-        <v>5</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -1175,10 +1175,10 @@
         <v>5</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D27" s="1">
         <v>7</v>
@@ -1187,7 +1187,7 @@
         <v>7</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -1195,10 +1195,10 @@
         <v>2</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D28" s="1">
         <v>1</v>
@@ -1207,7 +1207,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -1215,19 +1215,19 @@
         <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1">
+        <v>2</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1</v>
-      </c>
-      <c r="E29" s="1">
-        <v>2</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -1235,10 +1235,10 @@
         <v>2</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D30" s="1">
         <v>2</v>
@@ -1247,7 +1247,7 @@
         <v>4</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -1255,10 +1255,10 @@
         <v>3</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D31" s="1">
         <v>9</v>
@@ -1267,7 +1267,7 @@
         <v>9</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -1275,10 +1275,10 @@
         <v>5</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D32" s="1">
         <v>5</v>
@@ -1287,7 +1287,7 @@
         <v>6</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -1295,10 +1295,10 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D33" s="1">
         <v>5</v>
@@ -1307,7 +1307,7 @@
         <v>2</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>